<commit_message>
forgot to save a change
</commit_message>
<xml_diff>
--- a/CSV_Method/CenturyPlan_formatted.xlsx
+++ b/CSV_Method/CenturyPlan_formatted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\gtnash\repos\AmPowerGuide\CSV_Method\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4A64BE-B910-4D0D-B905-272827EDA823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD104CC0-9645-412F-9C92-2588BA75FB29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840" activeTab="2" xr2:uid="{5477C7E2-8D94-434C-9C36-5F567177BAE4}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="21705" activeTab="1" xr2:uid="{5477C7E2-8D94-434C-9C36-5F567177BAE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Formatted" sheetId="1" r:id="rId1"/>
@@ -1358,7 +1358,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>31</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>32</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>33</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>34</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>35</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>36</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>37</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <v>38</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <v>39</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <v>40</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <v>41</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <v>42</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <v>43</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <v>44</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <v>45</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
         <v>46</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
         <v>47</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <v>48</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <v>49</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <v>50</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <v>51</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="6">
         <v>52</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
         <v>53</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
         <v>54</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
         <v>55</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="6">
         <v>56</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="6">
         <v>57</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="6">
         <v>58</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="6">
         <v>59</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="6">
         <v>60</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="6">
         <v>61</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6">
         <v>62</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="6">
         <v>63</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="6">
         <v>64</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="6">
         <v>65</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="6">
         <v>66</v>
       </c>
@@ -2894,7 +2894,7 @@
       <c r="F69" s="9"/>
       <c r="G69" s="6"/>
     </row>
-    <row r="70" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
       <c r="C70" s="7"/>
@@ -2912,7 +2912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E313E52-A239-45A4-BF15-156E79F86F5E}">
   <dimension ref="A1:L133"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
@@ -3038,8 +3038,8 @@
         <v>240</v>
       </c>
       <c r="L3">
-        <f>1318/318</f>
-        <v>4.1446540880503147</v>
+        <f>100/L1</f>
+        <v>0.32467532467532467</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
@@ -5448,8 +5448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FFEF87C-6B05-48F7-9DAC-5E64FAA08DC7}">
   <dimension ref="A1:BK76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10:W75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6174,7 +6174,7 @@
       </c>
       <c r="K10" s="11">
         <f>'In Numbers'!E2*0.95*'In Numbers'!$L$3</f>
-        <v>748.11006289308182</v>
+        <v>58.603896103896105</v>
       </c>
       <c r="L10" t="s">
         <v>286</v>
@@ -6184,7 +6184,7 @@
       </c>
       <c r="N10" s="11">
         <f>'In Numbers'!E2*1.05*'In Numbers'!$L$3</f>
-        <v>826.85849056603774</v>
+        <v>64.772727272727266</v>
       </c>
       <c r="O10" t="s">
         <v>286</v>
@@ -6205,7 +6205,7 @@
         <v>233</v>
       </c>
       <c r="W10">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y10" t="s">
         <v>234</v>
@@ -6242,14 +6242,14 @@
       </c>
       <c r="K11" s="11">
         <f>'In Numbers'!E3*0.95*'In Numbers'!$L$3</f>
-        <v>641.79968553459116</v>
+        <v>50.275974025974023</v>
       </c>
       <c r="M11" t="s">
         <v>225</v>
       </c>
       <c r="N11" s="11">
         <f>'In Numbers'!E3*1.05*'In Numbers'!$L$3</f>
-        <v>709.35754716981137</v>
+        <v>55.56818181818182</v>
       </c>
       <c r="P11" t="s">
         <v>227</v>
@@ -6267,7 +6267,7 @@
         <v>233</v>
       </c>
       <c r="W11">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y11" t="s">
         <v>234</v>
@@ -6304,14 +6304,14 @@
       </c>
       <c r="K12" s="11">
         <f>'In Numbers'!E4*0.95*'In Numbers'!$L$3</f>
-        <v>736.29779874213841</v>
+        <v>57.678571428571431</v>
       </c>
       <c r="M12" t="s">
         <v>225</v>
       </c>
       <c r="N12" s="11">
         <f>'In Numbers'!E4*1.05*'In Numbers'!$L$3</f>
-        <v>813.80283018867931</v>
+        <v>63.75</v>
       </c>
       <c r="P12" t="s">
         <v>227</v>
@@ -6329,7 +6329,7 @@
         <v>233</v>
       </c>
       <c r="W12">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y12" t="s">
         <v>234</v>
@@ -6366,14 +6366,14 @@
       </c>
       <c r="K13" s="11">
         <f>'In Numbers'!E5*0.95*'In Numbers'!$L$3</f>
-        <v>641.79968553459116</v>
+        <v>50.275974025974023</v>
       </c>
       <c r="M13" t="s">
         <v>225</v>
       </c>
       <c r="N13" s="11">
         <f>'In Numbers'!E5*1.05*'In Numbers'!$L$3</f>
-        <v>709.35754716981137</v>
+        <v>55.56818181818182</v>
       </c>
       <c r="P13" t="s">
         <v>227</v>
@@ -6391,7 +6391,7 @@
         <v>233</v>
       </c>
       <c r="W13">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y13" t="s">
         <v>234</v>
@@ -6428,14 +6428,14 @@
       </c>
       <c r="K14" s="11">
         <f>'In Numbers'!E6*0.95*'In Numbers'!$L$3</f>
-        <v>759.92232704402522</v>
+        <v>59.529220779220779</v>
       </c>
       <c r="M14" t="s">
         <v>225</v>
       </c>
       <c r="N14" s="11">
         <f>'In Numbers'!E6*1.05*'In Numbers'!$L$3</f>
-        <v>839.91415094339629</v>
+        <v>65.795454545454547</v>
       </c>
       <c r="P14" t="s">
         <v>227</v>
@@ -6453,7 +6453,7 @@
         <v>233</v>
       </c>
       <c r="W14">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y14" t="s">
         <v>234</v>
@@ -6490,14 +6490,14 @@
       </c>
       <c r="K15" s="11">
         <f>'In Numbers'!E7*0.95*'In Numbers'!$L$3</f>
-        <v>807.17138364779873</v>
+        <v>63.230519480519483</v>
       </c>
       <c r="M15" t="s">
         <v>225</v>
       </c>
       <c r="N15" s="11">
         <f>'In Numbers'!E7*1.05*'In Numbers'!$L$3</f>
-        <v>892.13679245283026</v>
+        <v>69.88636363636364</v>
       </c>
       <c r="P15" t="s">
         <v>227</v>
@@ -6515,7 +6515,7 @@
         <v>233</v>
       </c>
       <c r="W15">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y15" t="s">
         <v>234</v>
@@ -6552,14 +6552,14 @@
       </c>
       <c r="K16" s="11">
         <f>'In Numbers'!E8*0.95*'In Numbers'!$L$3</f>
-        <v>755.98490566037731</v>
+        <v>59.220779220779214</v>
       </c>
       <c r="M16" t="s">
         <v>225</v>
       </c>
       <c r="N16" s="11">
         <f>'In Numbers'!E8*1.05*'In Numbers'!$L$3</f>
-        <v>835.56226415094352</v>
+        <v>65.454545454545467</v>
       </c>
       <c r="P16" t="s">
         <v>227</v>
@@ -6577,7 +6577,7 @@
         <v>233</v>
       </c>
       <c r="W16">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y16" t="s">
         <v>234</v>
@@ -6614,14 +6614,14 @@
       </c>
       <c r="K17" s="11">
         <f>'In Numbers'!E9*0.95*'In Numbers'!$L$3</f>
-        <v>637.86226415094347</v>
+        <v>49.967532467532472</v>
       </c>
       <c r="M17" t="s">
         <v>225</v>
       </c>
       <c r="N17" s="11">
         <f>'In Numbers'!E9*1.05*'In Numbers'!$L$3</f>
-        <v>705.00566037735848</v>
+        <v>55.227272727272727</v>
       </c>
       <c r="P17" t="s">
         <v>227</v>
@@ -6639,7 +6639,7 @@
         <v>233</v>
       </c>
       <c r="W17">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y17" t="s">
         <v>234</v>
@@ -6676,14 +6676,14 @@
       </c>
       <c r="K18" s="11">
         <f>'In Numbers'!E10*0.95*'In Numbers'!$L$3</f>
-        <v>716.6106918238994</v>
+        <v>56.13636363636364</v>
       </c>
       <c r="M18" t="s">
         <v>225</v>
       </c>
       <c r="N18" s="11">
         <f>'In Numbers'!E10*1.05*'In Numbers'!$L$3</f>
-        <v>792.0433962264151</v>
+        <v>62.04545454545454</v>
       </c>
       <c r="P18" t="s">
         <v>227</v>
@@ -6701,7 +6701,7 @@
         <v>233</v>
       </c>
       <c r="W18">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y18" t="s">
         <v>234</v>
@@ -6738,14 +6738,14 @@
       </c>
       <c r="K19" s="11">
         <f>'In Numbers'!E11*0.95*'In Numbers'!$L$3</f>
-        <v>740.23522012578621</v>
+        <v>57.987012987012982</v>
       </c>
       <c r="M19" t="s">
         <v>225</v>
       </c>
       <c r="N19" s="11">
         <f>'In Numbers'!E11*1.05*'In Numbers'!$L$3</f>
-        <v>818.15471698113208</v>
+        <v>64.090909090909093</v>
       </c>
       <c r="P19" t="s">
         <v>227</v>
@@ -6763,7 +6763,7 @@
         <v>233</v>
       </c>
       <c r="W19">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y19" t="s">
         <v>234</v>
@@ -6800,14 +6800,14 @@
       </c>
       <c r="K20" s="11">
         <f>'In Numbers'!E12*0.95*'In Numbers'!$L$3</f>
-        <v>649.67452830188677</v>
+        <v>50.892857142857146</v>
       </c>
       <c r="M20" t="s">
         <v>225</v>
       </c>
       <c r="N20" s="11">
         <f>'In Numbers'!E12*1.05*'In Numbers'!$L$3</f>
-        <v>718.06132075471703</v>
+        <v>56.25</v>
       </c>
       <c r="P20" t="s">
         <v>227</v>
@@ -6825,7 +6825,7 @@
         <v>233</v>
       </c>
       <c r="W20">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y20" t="s">
         <v>234</v>
@@ -6862,14 +6862,14 @@
       </c>
       <c r="K21" s="11">
         <f>'In Numbers'!E13*0.95*'In Numbers'!$L$3</f>
-        <v>799.29654088050313</v>
+        <v>62.61363636363636</v>
       </c>
       <c r="M21" t="s">
         <v>225</v>
       </c>
       <c r="N21" s="11">
         <f>'In Numbers'!E13*1.05*'In Numbers'!$L$3</f>
-        <v>883.4330188679246</v>
+        <v>69.204545454545453</v>
       </c>
       <c r="P21" t="s">
         <v>227</v>
@@ -6887,7 +6887,7 @@
         <v>233</v>
       </c>
       <c r="W21">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y21" t="s">
         <v>234</v>
@@ -6924,14 +6924,14 @@
       </c>
       <c r="K22" s="11">
         <f>'In Numbers'!E14*0.95*'In Numbers'!$L$3</f>
-        <v>645.73710691823896</v>
+        <v>50.584415584415581</v>
       </c>
       <c r="M22" t="s">
         <v>225</v>
       </c>
       <c r="N22" s="11">
         <f>'In Numbers'!E14*1.05*'In Numbers'!$L$3</f>
-        <v>713.70943396226426</v>
+        <v>55.909090909090914</v>
       </c>
       <c r="P22" t="s">
         <v>227</v>
@@ -6949,7 +6949,7 @@
         <v>233</v>
       </c>
       <c r="W22">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y22" t="s">
         <v>234</v>
@@ -6986,14 +6986,14 @@
       </c>
       <c r="K23" s="11">
         <f>'In Numbers'!E15*0.95*'In Numbers'!$L$3</f>
-        <v>728.42295597484281</v>
+        <v>57.061688311688314</v>
       </c>
       <c r="M23" t="s">
         <v>225</v>
       </c>
       <c r="N23" s="11">
         <f>'In Numbers'!E15*1.05*'In Numbers'!$L$3</f>
-        <v>805.09905660377365</v>
+        <v>63.06818181818182</v>
       </c>
       <c r="P23" t="s">
         <v>227</v>
@@ -7011,7 +7011,7 @@
         <v>233</v>
       </c>
       <c r="W23">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y23" t="s">
         <v>234</v>
@@ -7048,14 +7048,14 @@
       </c>
       <c r="K24" s="11">
         <f>'In Numbers'!E16*0.95*'In Numbers'!$L$3</f>
-        <v>791.42169811320753</v>
+        <v>61.996753246753244</v>
       </c>
       <c r="M24" t="s">
         <v>225</v>
       </c>
       <c r="N24" s="11">
         <f>'In Numbers'!E16*1.05*'In Numbers'!$L$3</f>
-        <v>874.72924528301894</v>
+        <v>68.52272727272728</v>
       </c>
       <c r="P24" t="s">
         <v>227</v>
@@ -7073,7 +7073,7 @@
         <v>233</v>
       </c>
       <c r="W24">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y24" t="s">
         <v>234</v>
@@ -7110,14 +7110,14 @@
       </c>
       <c r="K25" s="11">
         <f>'In Numbers'!E17*0.95*'In Numbers'!$L$3</f>
-        <v>685.11132075471698</v>
+        <v>53.668831168831161</v>
       </c>
       <c r="M25" t="s">
         <v>225</v>
       </c>
       <c r="N25" s="11">
         <f>'In Numbers'!E17*1.05*'In Numbers'!$L$3</f>
-        <v>757.22830188679256</v>
+        <v>59.31818181818182</v>
       </c>
       <c r="P25" t="s">
         <v>227</v>
@@ -7135,7 +7135,7 @@
         <v>233</v>
       </c>
       <c r="W25">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y25" t="s">
         <v>234</v>
@@ -7172,14 +7172,14 @@
       </c>
       <c r="K26" s="11">
         <f>'In Numbers'!E18*0.95*'In Numbers'!$L$3</f>
-        <v>815.04622641509434</v>
+        <v>63.847402597402592</v>
       </c>
       <c r="M26" t="s">
         <v>225</v>
       </c>
       <c r="N26" s="11">
         <f>'In Numbers'!E18*1.05*'In Numbers'!$L$3</f>
-        <v>900.84056603773604</v>
+        <v>70.568181818181827</v>
       </c>
       <c r="P26" t="s">
         <v>227</v>
@@ -7197,7 +7197,7 @@
         <v>233</v>
       </c>
       <c r="W26">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y26" t="s">
         <v>234</v>
@@ -7234,14 +7234,14 @@
       </c>
       <c r="K27" s="11">
         <f>'In Numbers'!E19*0.95*'In Numbers'!$L$3</f>
-        <v>704.79842767295588</v>
+        <v>55.211038961038952</v>
       </c>
       <c r="M27" t="s">
         <v>225</v>
       </c>
       <c r="N27" s="11">
         <f>'In Numbers'!E19*1.05*'In Numbers'!$L$3</f>
-        <v>778.98773584905666</v>
+        <v>61.02272727272728</v>
       </c>
       <c r="P27" t="s">
         <v>227</v>
@@ -7259,7 +7259,7 @@
         <v>233</v>
       </c>
       <c r="W27">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y27" t="s">
         <v>234</v>
@@ -7296,14 +7296,14 @@
       </c>
       <c r="K28" s="11">
         <f>'In Numbers'!E20*0.95*'In Numbers'!$L$3</f>
-        <v>838.67075471698115</v>
+        <v>65.69805194805194</v>
       </c>
       <c r="M28" t="s">
         <v>225</v>
       </c>
       <c r="N28" s="11">
         <f>'In Numbers'!E20*1.05*'In Numbers'!$L$3</f>
-        <v>926.95188679245291</v>
+        <v>72.61363636363636</v>
       </c>
       <c r="P28" t="s">
         <v>227</v>
@@ -7321,7 +7321,7 @@
         <v>233</v>
       </c>
       <c r="W28">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y28" t="s">
         <v>234</v>
@@ -7358,14 +7358,14 @@
       </c>
       <c r="K29" s="11">
         <f>'In Numbers'!E21*0.95*'In Numbers'!$L$3</f>
-        <v>728.42295597484281</v>
+        <v>57.061688311688314</v>
       </c>
       <c r="M29" t="s">
         <v>225</v>
       </c>
       <c r="N29" s="11">
         <f>'In Numbers'!E21*1.05*'In Numbers'!$L$3</f>
-        <v>805.09905660377365</v>
+        <v>63.06818181818182</v>
       </c>
       <c r="P29" t="s">
         <v>227</v>
@@ -7383,7 +7383,7 @@
         <v>233</v>
       </c>
       <c r="W29">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y29" t="s">
         <v>234</v>
@@ -7420,14 +7420,14 @@
       </c>
       <c r="K30" s="11">
         <f>'In Numbers'!E22*0.95*'In Numbers'!$L$3</f>
-        <v>779.60943396226412</v>
+        <v>61.071428571428569</v>
       </c>
       <c r="M30" t="s">
         <v>225</v>
       </c>
       <c r="N30" s="11">
         <f>'In Numbers'!E22*1.05*'In Numbers'!$L$3</f>
-        <v>861.67358490566039</v>
+        <v>67.5</v>
       </c>
       <c r="P30" t="s">
         <v>227</v>
@@ -7445,7 +7445,7 @@
         <v>233</v>
       </c>
       <c r="W30">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y30" t="s">
         <v>234</v>
@@ -7482,14 +7482,14 @@
       </c>
       <c r="K31" s="11">
         <f>'In Numbers'!E23*0.95*'In Numbers'!$L$3</f>
-        <v>563.05125786163524</v>
+        <v>44.107142857142854</v>
       </c>
       <c r="M31" t="s">
         <v>225</v>
       </c>
       <c r="N31" s="11">
         <f>'In Numbers'!E23*1.05*'In Numbers'!$L$3</f>
-        <v>622.31981132075475</v>
+        <v>48.75</v>
       </c>
       <c r="P31" t="s">
         <v>227</v>
@@ -7507,7 +7507,7 @@
         <v>233</v>
       </c>
       <c r="W31">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y31" t="s">
         <v>234</v>
@@ -7544,14 +7544,14 @@
       </c>
       <c r="K32" s="11">
         <f>'In Numbers'!E24*0.95*'In Numbers'!$L$3</f>
-        <v>811.10880503144654</v>
+        <v>63.538961038961034</v>
       </c>
       <c r="M32" t="s">
         <v>225</v>
       </c>
       <c r="N32" s="11">
         <f>'In Numbers'!E24*1.05*'In Numbers'!$L$3</f>
-        <v>896.48867924528315</v>
+        <v>70.227272727272734</v>
       </c>
       <c r="P32" t="s">
         <v>227</v>
@@ -7569,7 +7569,7 @@
         <v>233</v>
       </c>
       <c r="W32">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y32" t="s">
         <v>234</v>
@@ -7606,14 +7606,14 @@
       </c>
       <c r="K33" s="11">
         <f>'In Numbers'!E25*0.95*'In Numbers'!$L$3</f>
-        <v>692.98616352201259</v>
+        <v>54.285714285714285</v>
       </c>
       <c r="M33" t="s">
         <v>225</v>
       </c>
       <c r="N33" s="11">
         <f>'In Numbers'!E25*1.05*'In Numbers'!$L$3</f>
-        <v>765.93207547169823</v>
+        <v>60</v>
       </c>
       <c r="P33" t="s">
         <v>227</v>
@@ -7631,7 +7631,7 @@
         <v>233</v>
       </c>
       <c r="W33">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y33" t="s">
         <v>234</v>
@@ -7668,14 +7668,14 @@
       </c>
       <c r="K34" s="11">
         <f>'In Numbers'!E26*0.95*'In Numbers'!$L$3</f>
-        <v>818.98364779874214</v>
+        <v>64.15584415584415</v>
       </c>
       <c r="M34" t="s">
         <v>225</v>
       </c>
       <c r="N34" s="11">
         <f>'In Numbers'!E26*1.05*'In Numbers'!$L$3</f>
-        <v>905.1924528301887</v>
+        <v>70.909090909090907</v>
       </c>
       <c r="P34" t="s">
         <v>227</v>
@@ -7693,7 +7693,7 @@
         <v>233</v>
       </c>
       <c r="W34">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y34" t="s">
         <v>234</v>
@@ -7730,14 +7730,14 @@
       </c>
       <c r="K35" s="11">
         <f>'In Numbers'!E27*0.95*'In Numbers'!$L$3</f>
-        <v>681.17389937106918</v>
+        <v>53.36038961038961</v>
       </c>
       <c r="M35" t="s">
         <v>225</v>
       </c>
       <c r="N35" s="11">
         <f>'In Numbers'!E27*1.05*'In Numbers'!$L$3</f>
-        <v>752.87641509433968</v>
+        <v>58.977272727272727</v>
       </c>
       <c r="P35" t="s">
         <v>227</v>
@@ -7755,7 +7755,7 @@
         <v>233</v>
       </c>
       <c r="W35">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y35" t="s">
         <v>234</v>
@@ -7792,14 +7792,14 @@
       </c>
       <c r="K36" s="11">
         <f>'In Numbers'!E28*0.95*'In Numbers'!$L$3</f>
-        <v>815.04622641509434</v>
+        <v>63.847402597402592</v>
       </c>
       <c r="M36" t="s">
         <v>225</v>
       </c>
       <c r="N36" s="11">
         <f>'In Numbers'!E28*1.05*'In Numbers'!$L$3</f>
-        <v>900.84056603773604</v>
+        <v>70.568181818181827</v>
       </c>
       <c r="P36" t="s">
         <v>227</v>
@@ -7817,7 +7817,7 @@
         <v>233</v>
       </c>
       <c r="W36">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y36" t="s">
         <v>234</v>
@@ -7854,14 +7854,14 @@
       </c>
       <c r="K37" s="11">
         <f>'In Numbers'!E29*0.95*'In Numbers'!$L$3</f>
-        <v>673.29905660377358</v>
+        <v>52.743506493506487</v>
       </c>
       <c r="M37" t="s">
         <v>225</v>
       </c>
       <c r="N37" s="11">
         <f>'In Numbers'!E29*1.05*'In Numbers'!$L$3</f>
-        <v>744.17264150943402</v>
+        <v>58.295454545454547</v>
       </c>
       <c r="P37" t="s">
         <v>227</v>
@@ -7879,7 +7879,7 @@
         <v>233</v>
       </c>
       <c r="W37">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y37" t="s">
         <v>234</v>
@@ -7916,14 +7916,14 @@
       </c>
       <c r="K38" s="11">
         <f>'In Numbers'!E30*0.95*'In Numbers'!$L$3</f>
-        <v>771.73459119496852</v>
+        <v>60.454545454545453</v>
       </c>
       <c r="M38" t="s">
         <v>225</v>
       </c>
       <c r="N38" s="11">
         <f>'In Numbers'!E30*1.05*'In Numbers'!$L$3</f>
-        <v>852.96981132075484</v>
+        <v>66.818181818181827</v>
       </c>
       <c r="P38" t="s">
         <v>227</v>
@@ -7941,7 +7941,7 @@
         <v>233</v>
       </c>
       <c r="W38">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y38" t="s">
         <v>234</v>
@@ -7978,14 +7978,14 @@
       </c>
       <c r="K39" s="11">
         <f>'In Numbers'!E31*0.95*'In Numbers'!$L$3</f>
-        <v>724.48553459119489</v>
+        <v>56.753246753246749</v>
       </c>
       <c r="M39" t="s">
         <v>225</v>
       </c>
       <c r="N39" s="11">
         <f>'In Numbers'!E31*1.05*'In Numbers'!$L$3</f>
-        <v>800.74716981132087</v>
+        <v>62.727272727272734</v>
       </c>
       <c r="P39" t="s">
         <v>227</v>
@@ -8003,7 +8003,7 @@
         <v>233</v>
       </c>
       <c r="W39">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y39" t="s">
         <v>234</v>
@@ -8040,14 +8040,14 @@
       </c>
       <c r="K40" s="11">
         <f>'In Numbers'!E32*0.95*'In Numbers'!$L$3</f>
-        <v>807.17138364779873</v>
+        <v>63.230519480519483</v>
       </c>
       <c r="M40" t="s">
         <v>225</v>
       </c>
       <c r="N40" s="11">
         <f>'In Numbers'!E32*1.05*'In Numbers'!$L$3</f>
-        <v>892.13679245283026</v>
+        <v>69.88636363636364</v>
       </c>
       <c r="P40" t="s">
         <v>227</v>
@@ -8065,7 +8065,7 @@
         <v>233</v>
       </c>
       <c r="W40">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y40" t="s">
         <v>234</v>
@@ -8102,14 +8102,14 @@
       </c>
       <c r="K41" s="11">
         <f>'In Numbers'!E33*0.95*'In Numbers'!$L$3</f>
-        <v>685.11132075471698</v>
+        <v>53.668831168831161</v>
       </c>
       <c r="M41" t="s">
         <v>225</v>
       </c>
       <c r="N41" s="11">
         <f>'In Numbers'!E33*1.05*'In Numbers'!$L$3</f>
-        <v>757.22830188679256</v>
+        <v>59.31818181818182</v>
       </c>
       <c r="P41" t="s">
         <v>227</v>
@@ -8127,7 +8127,7 @@
         <v>233</v>
       </c>
       <c r="W41">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y41" t="s">
         <v>234</v>
@@ -8164,14 +8164,14 @@
       </c>
       <c r="K42" s="11">
         <f>'In Numbers'!E34*0.95*'In Numbers'!$L$3</f>
-        <v>799.29654088050313</v>
+        <v>62.61363636363636</v>
       </c>
       <c r="M42" t="s">
         <v>225</v>
       </c>
       <c r="N42" s="11">
         <f>'In Numbers'!E34*1.05*'In Numbers'!$L$3</f>
-        <v>883.4330188679246</v>
+        <v>69.204545454545453</v>
       </c>
       <c r="P42" t="s">
         <v>227</v>
@@ -8189,7 +8189,7 @@
         <v>233</v>
       </c>
       <c r="W42">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y42" t="s">
         <v>234</v>
@@ -8226,14 +8226,14 @@
       </c>
       <c r="K43" s="11">
         <f>'In Numbers'!E35*0.95*'In Numbers'!$L$3</f>
-        <v>720.5481132075472</v>
+        <v>56.444805194805191</v>
       </c>
       <c r="M43" t="s">
         <v>225</v>
       </c>
       <c r="N43" s="11">
         <f>'In Numbers'!E35*1.05*'In Numbers'!$L$3</f>
-        <v>796.39528301886799</v>
+        <v>62.38636363636364</v>
       </c>
       <c r="P43" t="s">
         <v>227</v>
@@ -8251,7 +8251,7 @@
         <v>233</v>
       </c>
       <c r="W43">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y43" t="s">
         <v>234</v>
@@ -8288,14 +8288,14 @@
       </c>
       <c r="K44" s="11">
         <f>'In Numbers'!E36*0.95*'In Numbers'!$L$3</f>
-        <v>3.9374213836477989</v>
+        <v>0.30844155844155841</v>
       </c>
       <c r="M44" t="s">
         <v>225</v>
       </c>
       <c r="N44" s="11">
         <f>'In Numbers'!E36*1.05*'In Numbers'!$L$3</f>
-        <v>4.3518867924528308</v>
+        <v>0.34090909090909094</v>
       </c>
       <c r="P44" t="s">
         <v>227</v>
@@ -8313,7 +8313,7 @@
         <v>233</v>
       </c>
       <c r="W44">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y44" t="s">
         <v>234</v>
@@ -8350,14 +8350,14 @@
       </c>
       <c r="K45" s="11">
         <f>'In Numbers'!E37*0.95*'In Numbers'!$L$3</f>
-        <v>728.42295597484281</v>
+        <v>57.061688311688314</v>
       </c>
       <c r="M45" t="s">
         <v>225</v>
       </c>
       <c r="N45" s="11">
         <f>'In Numbers'!E37*1.05*'In Numbers'!$L$3</f>
-        <v>805.09905660377365</v>
+        <v>63.06818181818182</v>
       </c>
       <c r="P45" t="s">
         <v>227</v>
@@ -8375,7 +8375,7 @@
         <v>233</v>
       </c>
       <c r="W45">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y45" t="s">
         <v>234</v>
@@ -8412,14 +8412,14 @@
       </c>
       <c r="K46" s="11">
         <f>'In Numbers'!E38*0.95*'In Numbers'!$L$3</f>
-        <v>1039.4792452830188</v>
+        <v>81.428571428571416</v>
       </c>
       <c r="M46" t="s">
         <v>225</v>
       </c>
       <c r="N46" s="11">
         <f>'In Numbers'!E38*1.05*'In Numbers'!$L$3</f>
-        <v>1148.8981132075471</v>
+        <v>90</v>
       </c>
       <c r="P46" t="s">
         <v>227</v>
@@ -8437,7 +8437,7 @@
         <v>233</v>
       </c>
       <c r="W46">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y46" t="s">
         <v>234</v>
@@ -8474,14 +8474,14 @@
       </c>
       <c r="K47" s="11">
         <f>'In Numbers'!E39*0.95*'In Numbers'!$L$3</f>
-        <v>811.10880503144654</v>
+        <v>63.538961038961034</v>
       </c>
       <c r="M47" t="s">
         <v>225</v>
       </c>
       <c r="N47" s="11">
         <f>'In Numbers'!E39*1.05*'In Numbers'!$L$3</f>
-        <v>896.48867924528315</v>
+        <v>70.227272727272734</v>
       </c>
       <c r="P47" t="s">
         <v>227</v>
@@ -8499,7 +8499,7 @@
         <v>233</v>
       </c>
       <c r="W47">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y47" t="s">
         <v>234</v>
@@ -8536,14 +8536,14 @@
       </c>
       <c r="K48" s="11">
         <f>'In Numbers'!E40*0.95*'In Numbers'!$L$3</f>
-        <v>460.67830188679244</v>
+        <v>36.087662337662337</v>
       </c>
       <c r="M48" t="s">
         <v>225</v>
       </c>
       <c r="N48" s="11">
         <f>'In Numbers'!E40*1.05*'In Numbers'!$L$3</f>
-        <v>509.17075471698121</v>
+        <v>39.88636363636364</v>
       </c>
       <c r="P48" t="s">
         <v>227</v>
@@ -8561,7 +8561,7 @@
         <v>233</v>
       </c>
       <c r="W48">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y48" t="s">
         <v>234</v>
@@ -8598,14 +8598,14 @@
       </c>
       <c r="K49" s="11">
         <f>'In Numbers'!E41*0.95*'In Numbers'!$L$3</f>
-        <v>826.85849056603774</v>
+        <v>64.772727272727266</v>
       </c>
       <c r="M49" t="s">
         <v>225</v>
       </c>
       <c r="N49" s="11">
         <f>'In Numbers'!E41*1.05*'In Numbers'!$L$3</f>
-        <v>913.89622641509436</v>
+        <v>71.590909090909093</v>
       </c>
       <c r="P49" t="s">
         <v>227</v>
@@ -8623,7 +8623,7 @@
         <v>233</v>
       </c>
       <c r="W49">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y49" t="s">
         <v>234</v>
@@ -8660,14 +8660,14 @@
       </c>
       <c r="K50" s="11">
         <f>'In Numbers'!E42*0.95*'In Numbers'!$L$3</f>
-        <v>653.61194968553457</v>
+        <v>51.201298701298697</v>
       </c>
       <c r="M50" t="s">
         <v>225</v>
       </c>
       <c r="N50" s="11">
         <f>'In Numbers'!E42*1.05*'In Numbers'!$L$3</f>
-        <v>722.41320754716992</v>
+        <v>56.590909090909093</v>
       </c>
       <c r="P50" t="s">
         <v>227</v>
@@ -8685,7 +8685,7 @@
         <v>233</v>
       </c>
       <c r="W50">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y50" t="s">
         <v>234</v>
@@ -8722,14 +8722,14 @@
       </c>
       <c r="K51" s="11">
         <f>'In Numbers'!E43*0.95*'In Numbers'!$L$3</f>
-        <v>905.60691823899379</v>
+        <v>70.941558441558442</v>
       </c>
       <c r="M51" t="s">
         <v>225</v>
       </c>
       <c r="N51" s="11">
         <f>'In Numbers'!E43*1.05*'In Numbers'!$L$3</f>
-        <v>1000.933962264151</v>
+        <v>78.409090909090907</v>
       </c>
       <c r="P51" t="s">
         <v>227</v>
@@ -8747,7 +8747,7 @@
         <v>233</v>
       </c>
       <c r="W51">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y51" t="s">
         <v>234</v>
@@ -8784,14 +8784,14 @@
       </c>
       <c r="K52" s="11">
         <f>'In Numbers'!E44*0.95*'In Numbers'!$L$3</f>
-        <v>685.11132075471698</v>
+        <v>53.668831168831161</v>
       </c>
       <c r="M52" t="s">
         <v>225</v>
       </c>
       <c r="N52" s="11">
         <f>'In Numbers'!E44*1.05*'In Numbers'!$L$3</f>
-        <v>757.22830188679256</v>
+        <v>59.31818181818182</v>
       </c>
       <c r="P52" t="s">
         <v>227</v>
@@ -8809,7 +8809,7 @@
         <v>233</v>
       </c>
       <c r="W52">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y52" t="s">
         <v>234</v>
@@ -8846,14 +8846,14 @@
       </c>
       <c r="K53" s="11">
         <f>'In Numbers'!E45*0.95*'In Numbers'!$L$3</f>
-        <v>767.79716981132083</v>
+        <v>60.146103896103895</v>
       </c>
       <c r="M53" t="s">
         <v>225</v>
       </c>
       <c r="N53" s="11">
         <f>'In Numbers'!E45*1.05*'In Numbers'!$L$3</f>
-        <v>848.61792452830196</v>
+        <v>66.477272727272734</v>
       </c>
       <c r="P53" t="s">
         <v>227</v>
@@ -8871,7 +8871,7 @@
         <v>233</v>
       </c>
       <c r="W53">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y53" t="s">
         <v>234</v>
@@ -8908,14 +8908,14 @@
       </c>
       <c r="K54" s="11">
         <f>'In Numbers'!E46*0.95*'In Numbers'!$L$3</f>
-        <v>629.98742138364787</v>
+        <v>49.350649350649348</v>
       </c>
       <c r="M54" t="s">
         <v>225</v>
       </c>
       <c r="N54" s="11">
         <f>'In Numbers'!E46*1.05*'In Numbers'!$L$3</f>
-        <v>696.30188679245282</v>
+        <v>54.545454545454547</v>
       </c>
       <c r="P54" t="s">
         <v>227</v>
@@ -8933,7 +8933,7 @@
         <v>233</v>
       </c>
       <c r="W54">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y54" t="s">
         <v>234</v>
@@ -8970,14 +8970,14 @@
       </c>
       <c r="K55" s="11">
         <f>'In Numbers'!E47*0.95*'In Numbers'!$L$3</f>
-        <v>763.85974842767291</v>
+        <v>59.83766233766233</v>
       </c>
       <c r="M55" t="s">
         <v>225</v>
       </c>
       <c r="N55" s="11">
         <f>'In Numbers'!E47*1.05*'In Numbers'!$L$3</f>
-        <v>844.26603773584918</v>
+        <v>66.13636363636364</v>
       </c>
       <c r="P55" t="s">
         <v>227</v>
@@ -8995,7 +8995,7 @@
         <v>233</v>
       </c>
       <c r="W55">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y55" t="s">
         <v>234</v>
@@ -9032,14 +9032,14 @@
       </c>
       <c r="K56" s="11">
         <f>'In Numbers'!E48*0.95*'In Numbers'!$L$3</f>
-        <v>685.11132075471698</v>
+        <v>53.668831168831161</v>
       </c>
       <c r="M56" t="s">
         <v>225</v>
       </c>
       <c r="N56" s="11">
         <f>'In Numbers'!E48*1.05*'In Numbers'!$L$3</f>
-        <v>757.22830188679256</v>
+        <v>59.31818181818182</v>
       </c>
       <c r="P56" t="s">
         <v>227</v>
@@ -9057,7 +9057,7 @@
         <v>233</v>
       </c>
       <c r="W56">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y56" t="s">
         <v>234</v>
@@ -9094,14 +9094,14 @@
       </c>
       <c r="K57" s="11">
         <f>'In Numbers'!E49*0.95*'In Numbers'!$L$3</f>
-        <v>728.42295597484281</v>
+        <v>57.061688311688314</v>
       </c>
       <c r="M57" t="s">
         <v>225</v>
       </c>
       <c r="N57" s="11">
         <f>'In Numbers'!E49*1.05*'In Numbers'!$L$3</f>
-        <v>805.09905660377365</v>
+        <v>63.06818181818182</v>
       </c>
       <c r="P57" t="s">
         <v>227</v>
@@ -9119,7 +9119,7 @@
         <v>233</v>
       </c>
       <c r="W57">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y57" t="s">
         <v>234</v>
@@ -9156,14 +9156,14 @@
       </c>
       <c r="K58" s="11">
         <f>'In Numbers'!E50*0.95*'In Numbers'!$L$3</f>
-        <v>791.42169811320753</v>
+        <v>61.996753246753244</v>
       </c>
       <c r="M58" t="s">
         <v>225</v>
       </c>
       <c r="N58" s="11">
         <f>'In Numbers'!E50*1.05*'In Numbers'!$L$3</f>
-        <v>874.72924528301894</v>
+        <v>68.52272727272728</v>
       </c>
       <c r="P58" t="s">
         <v>227</v>
@@ -9181,7 +9181,7 @@
         <v>233</v>
       </c>
       <c r="W58">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y58" t="s">
         <v>234</v>
@@ -9218,14 +9218,14 @@
       </c>
       <c r="K59" s="11">
         <f>'In Numbers'!E51*0.95*'In Numbers'!$L$3</f>
-        <v>657.54937106918248</v>
+        <v>51.509740259740262</v>
       </c>
       <c r="M59" t="s">
         <v>225</v>
       </c>
       <c r="N59" s="11">
         <f>'In Numbers'!E51*1.05*'In Numbers'!$L$3</f>
-        <v>726.76509433962269</v>
+        <v>56.93181818181818</v>
       </c>
       <c r="P59" t="s">
         <v>227</v>
@@ -9243,7 +9243,7 @@
         <v>233</v>
       </c>
       <c r="W59">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y59" t="s">
         <v>234</v>
@@ -9280,14 +9280,14 @@
       </c>
       <c r="K60" s="11">
         <f>'In Numbers'!E52*0.95*'In Numbers'!$L$3</f>
-        <v>744.1726415094339</v>
+        <v>58.29545454545454</v>
       </c>
       <c r="M60" t="s">
         <v>225</v>
       </c>
       <c r="N60" s="11">
         <f>'In Numbers'!E52*1.05*'In Numbers'!$L$3</f>
-        <v>822.50660377358497</v>
+        <v>64.431818181818187</v>
       </c>
       <c r="P60" t="s">
         <v>227</v>
@@ -9305,7 +9305,7 @@
         <v>233</v>
       </c>
       <c r="W60">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y60" t="s">
         <v>234</v>
@@ -9342,14 +9342,14 @@
       </c>
       <c r="K61" s="11">
         <f>'In Numbers'!E53*0.95*'In Numbers'!$L$3</f>
-        <v>834.73333333333323</v>
+        <v>65.389610389610382</v>
       </c>
       <c r="M61" t="s">
         <v>225</v>
       </c>
       <c r="N61" s="11">
         <f>'In Numbers'!E53*1.05*'In Numbers'!$L$3</f>
-        <v>922.60000000000014</v>
+        <v>72.27272727272728</v>
       </c>
       <c r="P61" t="s">
         <v>227</v>
@@ -9367,7 +9367,7 @@
         <v>233</v>
       </c>
       <c r="W61">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y61" t="s">
         <v>234</v>
@@ -9404,14 +9404,14 @@
       </c>
       <c r="K62" s="11">
         <f>'In Numbers'!E54*0.95*'In Numbers'!$L$3</f>
-        <v>728.42295597484281</v>
+        <v>57.061688311688314</v>
       </c>
       <c r="M62" t="s">
         <v>225</v>
       </c>
       <c r="N62" s="11">
         <f>'In Numbers'!E54*1.05*'In Numbers'!$L$3</f>
-        <v>805.09905660377365</v>
+        <v>63.06818181818182</v>
       </c>
       <c r="P62" t="s">
         <v>227</v>
@@ -9429,7 +9429,7 @@
         <v>233</v>
       </c>
       <c r="W62">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y62" t="s">
         <v>234</v>
@@ -9466,14 +9466,14 @@
       </c>
       <c r="K63" s="11">
         <f>'In Numbers'!E55*0.95*'In Numbers'!$L$3</f>
-        <v>145.68459119496856</v>
+        <v>11.412337662337661</v>
       </c>
       <c r="M63" t="s">
         <v>225</v>
       </c>
       <c r="N63" s="11">
         <f>'In Numbers'!E55*1.05*'In Numbers'!$L$3</f>
-        <v>161.01981132075474</v>
+        <v>12.613636363636363</v>
       </c>
       <c r="P63" t="s">
         <v>227</v>
@@ -9491,7 +9491,7 @@
         <v>233</v>
       </c>
       <c r="W63">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y63" t="s">
         <v>234</v>
@@ -9528,14 +9528,14 @@
       </c>
       <c r="K64" s="11">
         <f>'In Numbers'!E56*0.95*'In Numbers'!$L$3</f>
-        <v>724.48553459119489</v>
+        <v>56.753246753246749</v>
       </c>
       <c r="M64" t="s">
         <v>225</v>
       </c>
       <c r="N64" s="11">
         <f>'In Numbers'!E56*1.05*'In Numbers'!$L$3</f>
-        <v>800.74716981132087</v>
+        <v>62.727272727272734</v>
       </c>
       <c r="P64" t="s">
         <v>227</v>
@@ -9553,7 +9553,7 @@
         <v>233</v>
       </c>
       <c r="W64">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y64" t="s">
         <v>234</v>
@@ -9590,14 +9590,14 @@
       </c>
       <c r="K65" s="11">
         <f>'In Numbers'!E57*0.95*'In Numbers'!$L$3</f>
-        <v>925.2940251572328</v>
+        <v>72.483766233766232</v>
       </c>
       <c r="M65" t="s">
         <v>225</v>
       </c>
       <c r="N65" s="11">
         <f>'In Numbers'!E57*1.05*'In Numbers'!$L$3</f>
-        <v>1022.6933962264152</v>
+        <v>80.11363636363636</v>
       </c>
       <c r="P65" t="s">
         <v>227</v>
@@ -9615,7 +9615,7 @@
         <v>233</v>
       </c>
       <c r="W65">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y65" t="s">
         <v>234</v>
@@ -9652,14 +9652,14 @@
       </c>
       <c r="K66" s="11">
         <f>'In Numbers'!E58*0.95*'In Numbers'!$L$3</f>
-        <v>720.5481132075472</v>
+        <v>56.444805194805191</v>
       </c>
       <c r="M66" t="s">
         <v>225</v>
       </c>
       <c r="N66" s="11">
         <f>'In Numbers'!E58*1.05*'In Numbers'!$L$3</f>
-        <v>796.39528301886799</v>
+        <v>62.38636363636364</v>
       </c>
       <c r="P66" t="s">
         <v>227</v>
@@ -9677,7 +9677,7 @@
         <v>233</v>
       </c>
       <c r="W66">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y66" t="s">
         <v>234</v>
@@ -9714,14 +9714,14 @@
       </c>
       <c r="K67" s="11">
         <f>'In Numbers'!E59*0.95*'In Numbers'!$L$3</f>
-        <v>582.73836477987425</v>
+        <v>45.649350649350644</v>
       </c>
       <c r="M67" t="s">
         <v>225</v>
       </c>
       <c r="N67" s="11">
         <f>'In Numbers'!E59*1.05*'In Numbers'!$L$3</f>
-        <v>644.07924528301896</v>
+        <v>50.454545454545453</v>
       </c>
       <c r="P67" t="s">
         <v>227</v>
@@ -9739,7 +9739,7 @@
         <v>233</v>
       </c>
       <c r="W67">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y67" t="s">
         <v>234</v>
@@ -9776,14 +9776,14 @@
       </c>
       <c r="K68" s="11">
         <f>'In Numbers'!E60*0.95*'In Numbers'!$L$3</f>
-        <v>791.42169811320753</v>
+        <v>61.996753246753244</v>
       </c>
       <c r="M68" t="s">
         <v>225</v>
       </c>
       <c r="N68" s="11">
         <f>'In Numbers'!E60*1.05*'In Numbers'!$L$3</f>
-        <v>874.72924528301894</v>
+        <v>68.52272727272728</v>
       </c>
       <c r="P68" t="s">
         <v>227</v>
@@ -9801,7 +9801,7 @@
         <v>233</v>
       </c>
       <c r="W68">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y68" t="s">
         <v>234</v>
@@ -9838,14 +9838,14 @@
       </c>
       <c r="K69" s="11">
         <f>'In Numbers'!E61*0.95*'In Numbers'!$L$3</f>
-        <v>712.6732704402516</v>
+        <v>55.827922077922075</v>
       </c>
       <c r="M69" t="s">
         <v>225</v>
       </c>
       <c r="N69" s="11">
         <f>'In Numbers'!E61*1.05*'In Numbers'!$L$3</f>
-        <v>787.69150943396232</v>
+        <v>61.70454545454546</v>
       </c>
       <c r="P69" t="s">
         <v>227</v>
@@ -9863,7 +9863,7 @@
         <v>233</v>
       </c>
       <c r="W69">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y69" t="s">
         <v>234</v>
@@ -9900,14 +9900,14 @@
       </c>
       <c r="K70" s="11">
         <f>'In Numbers'!E62*0.95*'In Numbers'!$L$3</f>
-        <v>673.29905660377358</v>
+        <v>52.743506493506487</v>
       </c>
       <c r="M70" t="s">
         <v>225</v>
       </c>
       <c r="N70" s="11">
         <f>'In Numbers'!E62*1.05*'In Numbers'!$L$3</f>
-        <v>744.17264150943402</v>
+        <v>58.295454545454547</v>
       </c>
       <c r="P70" t="s">
         <v>227</v>
@@ -9925,7 +9925,7 @@
         <v>233</v>
       </c>
       <c r="W70">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y70" t="s">
         <v>234</v>
@@ -9962,14 +9962,14 @@
       </c>
       <c r="K71" s="11">
         <f>'In Numbers'!E63*0.95*'In Numbers'!$L$3</f>
-        <v>736.29779874213841</v>
+        <v>57.678571428571431</v>
       </c>
       <c r="M71" t="s">
         <v>225</v>
       </c>
       <c r="N71" s="11">
         <f>'In Numbers'!E63*1.05*'In Numbers'!$L$3</f>
-        <v>813.80283018867931</v>
+        <v>63.75</v>
       </c>
       <c r="P71" t="s">
         <v>227</v>
@@ -9987,7 +9987,7 @@
         <v>233</v>
       </c>
       <c r="W71">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y71" t="s">
         <v>234</v>
@@ -10024,14 +10024,14 @@
       </c>
       <c r="K72" s="11">
         <f>'In Numbers'!E64*0.95*'In Numbers'!$L$3</f>
-        <v>921.35660377358488</v>
+        <v>72.175324675324674</v>
       </c>
       <c r="M72" t="s">
         <v>225</v>
       </c>
       <c r="N72" s="11">
         <f>'In Numbers'!E64*1.05*'In Numbers'!$L$3</f>
-        <v>1018.3415094339624</v>
+        <v>79.77272727272728</v>
       </c>
       <c r="P72" t="s">
         <v>227</v>
@@ -10049,7 +10049,7 @@
         <v>233</v>
       </c>
       <c r="W72">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y72" t="s">
         <v>234</v>
@@ -10086,14 +10086,14 @@
       </c>
       <c r="K73" s="11">
         <f>'In Numbers'!E65*0.95*'In Numbers'!$L$3</f>
-        <v>783.54685534591192</v>
+        <v>61.37987012987012</v>
       </c>
       <c r="M73" t="s">
         <v>225</v>
       </c>
       <c r="N73" s="11">
         <f>'In Numbers'!E65*1.05*'In Numbers'!$L$3</f>
-        <v>866.02547169811328</v>
+        <v>67.840909090909093</v>
       </c>
       <c r="P73" t="s">
         <v>227</v>
@@ -10111,7 +10111,7 @@
         <v>233</v>
       </c>
       <c r="W73">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y73" t="s">
         <v>234</v>
@@ -10148,14 +10148,14 @@
       </c>
       <c r="K74" s="11">
         <f>'In Numbers'!E66*0.95*'In Numbers'!$L$3</f>
-        <v>712.6732704402516</v>
+        <v>55.827922077922075</v>
       </c>
       <c r="M74" t="s">
         <v>225</v>
       </c>
       <c r="N74" s="11">
         <f>'In Numbers'!E66*1.05*'In Numbers'!$L$3</f>
-        <v>787.69150943396232</v>
+        <v>61.70454545454546</v>
       </c>
       <c r="P74" t="s">
         <v>227</v>
@@ -10173,7 +10173,7 @@
         <v>233</v>
       </c>
       <c r="W74">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y74" t="s">
         <v>234</v>
@@ -10210,14 +10210,14 @@
       </c>
       <c r="K75" s="11">
         <f>'In Numbers'!E67*0.95*'In Numbers'!$L$3</f>
-        <v>370.11761006289311</v>
+        <v>28.993506493506491</v>
       </c>
       <c r="M75" t="s">
         <v>225</v>
       </c>
       <c r="N75" s="11">
         <f>'In Numbers'!E67*1.05*'In Numbers'!$L$3</f>
-        <v>409.07735849056604</v>
+        <v>32.045454545454547</v>
       </c>
       <c r="P75" t="s">
         <v>227</v>
@@ -10235,7 +10235,7 @@
         <v>233</v>
       </c>
       <c r="W75">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Y75" t="s">
         <v>234</v>

</xml_diff>